<commit_message>
Fix file path for Render depoloyment
</commit_message>
<xml_diff>
--- a/SE_Gantt_Chart.xlsx
+++ b/SE_Gantt_Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29101"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29108"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ocortes\Desktop\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{CB6EDF8D-E397-4129-91FA-3AF6A7197BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF257AA9-A73A-4B20-B232-15DA07DCB24B}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{CB6EDF8D-E397-4129-91FA-3AF6A7197BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{649E3CB8-4A00-4666-9DAC-5E09BF08817A}"/>
   <bookViews>
     <workbookView xWindow="-4305" yWindow="-21720" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="117">
   <si>
     <t>Task</t>
   </si>
@@ -388,9 +388,6 @@
   </si>
   <si>
     <t>Taher Poonawala</t>
-  </si>
-  <si>
-    <t>TEST</t>
   </si>
 </sst>
 </file>
@@ -481,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -566,6 +563,7 @@
     <xf numFmtId="165" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -881,8 +879,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6F977E5F-6B86-4459-A6B5-2FEC550C34BB}" name="Table3" displayName="Table3" ref="A1:K94" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:K94" xr:uid="{6F977E5F-6B86-4459-A6B5-2FEC550C34BB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6F977E5F-6B86-4459-A6B5-2FEC550C34BB}" name="Table3" displayName="Table3" ref="A1:K96" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:K96" xr:uid="{6F977E5F-6B86-4459-A6B5-2FEC550C34BB}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{44585A81-5219-429F-B7FD-92B2CA790F1C}" name="Plant" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{989C4717-7A23-4A84-AA25-B16E5CA4B006}" name="Project Name" dataDxfId="8">
@@ -1408,10 +1406,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF4A40D-63A7-47A6-905A-C1FD60372FCA}">
-  <dimension ref="A1:K94"/>
+  <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4369,35 +4367,41 @@
       <c r="K93" s="22"/>
     </row>
     <row r="94" spans="1:11">
-      <c r="A94" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="B94" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="C94" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="D94" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="E94" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="F94" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="G94" t="s">
-        <v>117</v>
-      </c>
+      <c r="A94" s="26"/>
+      <c r="B94" s="27"/>
+      <c r="C94" s="28"/>
+      <c r="D94" s="28"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="28"/>
+      <c r="G94" s="30"/>
       <c r="H94" s="29"/>
-      <c r="I94" s="29">
-        <v>45658</v>
-      </c>
-      <c r="J94" s="17">
-        <v>45993</v>
-      </c>
+      <c r="I94" s="29"/>
+      <c r="J94" s="17"/>
       <c r="K94" s="18"/>
+    </row>
+    <row r="95" spans="1:11">
+      <c r="A95" s="26"/>
+      <c r="B95" s="27"/>
+      <c r="C95" s="28"/>
+      <c r="D95" s="28"/>
+      <c r="E95" s="5"/>
+      <c r="F95" s="28"/>
+      <c r="H95" s="29"/>
+      <c r="I95" s="29"/>
+      <c r="J95" s="17"/>
+      <c r="K95" s="18"/>
+    </row>
+    <row r="96" spans="1:11">
+      <c r="A96" s="26"/>
+      <c r="B96" s="27"/>
+      <c r="C96" s="28"/>
+      <c r="D96" s="28"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="28"/>
+      <c r="H96" s="29"/>
+      <c r="I96" s="29"/>
+      <c r="J96" s="17"/>
+      <c r="K96" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update to app and SE_Gantt_Chart
</commit_message>
<xml_diff>
--- a/SE_Gantt_Chart.xlsx
+++ b/SE_Gantt_Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ocortes\Desktop\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{CB6EDF8D-E397-4129-91FA-3AF6A7197BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{649E3CB8-4A00-4666-9DAC-5E09BF08817A}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{CB6EDF8D-E397-4129-91FA-3AF6A7197BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD93F352-E425-44C2-A47E-360B1C40A3A2}"/>
   <bookViews>
     <workbookView xWindow="-4305" yWindow="-21720" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="211">
   <si>
     <t>Task</t>
   </si>
@@ -141,6 +141,9 @@
     <t>JAX</t>
   </si>
   <si>
+    <t>JAX Additional 3PL</t>
+  </si>
+  <si>
     <t>1PL</t>
   </si>
   <si>
@@ -156,6 +159,9 @@
     <t>KC2</t>
   </si>
   <si>
+    <t>KC2 Dynamic Tilt Functionality Fix</t>
+  </si>
+  <si>
     <t>Ad Hoc</t>
   </si>
   <si>
@@ -168,15 +174,24 @@
     <t>LAN</t>
   </si>
   <si>
+    <t>LAN ATU Kit Addition for DA2 L5 WIP</t>
+  </si>
+  <si>
     <t>German Estrada-Gutierrez</t>
   </si>
   <si>
     <t>OKC</t>
   </si>
   <si>
+    <t>OKC Shipping Gaylord with LGV</t>
+  </si>
+  <si>
     <t>BLM</t>
   </si>
   <si>
+    <t>BLM Check In lane expansion</t>
+  </si>
+  <si>
     <t>Check in Lane Expansion</t>
   </si>
   <si>
@@ -186,45 +201,75 @@
     <t>RCH</t>
   </si>
   <si>
+    <t>RCH RCH Check-In Lane: Project Planning Phase</t>
+  </si>
+  <si>
     <t>KEN</t>
   </si>
   <si>
+    <t>KEN KEN -LAYOUT OPTIMIZATION</t>
+  </si>
+  <si>
     <t>Layout Modification</t>
   </si>
   <si>
     <t>MIL</t>
   </si>
   <si>
+    <t>MIL L3 (Aluminum Line)</t>
+  </si>
+  <si>
     <t>Line Additions</t>
   </si>
   <si>
     <t>HAZ</t>
   </si>
   <si>
+    <t>HAZ Layout Opt. (Removal PBC)</t>
+  </si>
+  <si>
     <t>Opt</t>
   </si>
   <si>
     <t>Mohammad Karlawala</t>
   </si>
   <si>
+    <t>JAX Layout Opt. (Removal PBC)</t>
+  </si>
+  <si>
     <t>RIA</t>
   </si>
   <si>
+    <t>RIA Layout Optimization</t>
+  </si>
+  <si>
     <t>Victor Arrizon</t>
   </si>
   <si>
+    <t>HAZ Implementation of Embedded</t>
+  </si>
+  <si>
     <t>Software Enhancement</t>
   </si>
   <si>
     <t>TEM</t>
   </si>
   <si>
+    <t>TEM E80 Reach Optimization (Multiple sites but starting in TEM)</t>
+  </si>
+  <si>
     <t>NIA</t>
   </si>
   <si>
+    <t>NIA weight Segregation roll out</t>
+  </si>
+  <si>
     <t>CIN</t>
   </si>
   <si>
+    <t>CIN S.M.I.L.E E80</t>
+  </si>
+  <si>
     <t>Software Update</t>
   </si>
   <si>
@@ -234,39 +279,81 @@
     <t>Henry Martinez</t>
   </si>
   <si>
+    <t>JAX Ambient Room Automation</t>
+  </si>
+  <si>
     <t>Yusuf Benton</t>
   </si>
   <si>
+    <t>NIA MA Cloud Development</t>
+  </si>
+  <si>
     <t>ST4</t>
   </si>
   <si>
+    <t>ST4 Triple Stack</t>
+  </si>
+  <si>
     <t>Triple Stack</t>
   </si>
   <si>
+    <t>JAX Dual Pallet Drive- In Racking</t>
+  </si>
+  <si>
     <t>Layout Mod</t>
   </si>
   <si>
     <t>LOU</t>
   </si>
   <si>
+    <t>LOU Layout Optimization</t>
+  </si>
+  <si>
+    <t>NIA LGV Sensor Obsolescence</t>
+  </si>
+  <si>
     <t>Jason rodriguez</t>
   </si>
   <si>
+    <t>NIA LGV Safety Campaign</t>
+  </si>
+  <si>
     <t>Safety</t>
   </si>
   <si>
+    <t>ST4 Dual pallet Drive- in Racking</t>
+  </si>
+  <si>
+    <t>NIA R&amp;D Sensor Retrofit Roll out - 1</t>
+  </si>
+  <si>
     <t>Cole Pellegrini</t>
   </si>
   <si>
+    <t>NIA R&amp;D Sensor Retrofit Roll out - 2</t>
+  </si>
+  <si>
     <t>DAL</t>
   </si>
   <si>
+    <t>DAL LGV Conversion</t>
+  </si>
+  <si>
     <t>9/726</t>
   </si>
   <si>
+    <t>NIA VP Line Optimization Roll Out</t>
+  </si>
+  <si>
+    <t>NIA VP Line Additiona (Line in a box)</t>
+  </si>
+  <si>
     <t>ST3</t>
   </si>
   <si>
+    <t>ST3 1PL</t>
+  </si>
+  <si>
     <t>Active</t>
   </si>
   <si>
@@ -276,15 +363,42 @@
     <t>BAY</t>
   </si>
   <si>
+    <t>BAY 3HX Exit (2 LGVs/ 3 ATU kits)</t>
+  </si>
+  <si>
     <t>Ricardo Garcia</t>
   </si>
   <si>
+    <t>KC2 KC2 Injection Tote Automation</t>
+  </si>
+  <si>
+    <t>LAN Layout Opt. (PBC Removal)</t>
+  </si>
+  <si>
     <t>N/A</t>
   </si>
   <si>
     <t>MXC</t>
   </si>
   <si>
+    <t>MXC Shipping Optimization</t>
+  </si>
+  <si>
+    <t>NIA CGR03544 NIA - WIP Pallets Modification</t>
+  </si>
+  <si>
+    <t>NIA Monthly SE KPI</t>
+  </si>
+  <si>
+    <t>NIA 0 LGV Alarms</t>
+  </si>
+  <si>
+    <t>NIA Master NIA OIL List</t>
+  </si>
+  <si>
+    <t>CIN BTS L1 - L3</t>
+  </si>
+  <si>
     <t>BTS</t>
   </si>
   <si>
@@ -294,6 +408,9 @@
     <t>GDL</t>
   </si>
   <si>
+    <t>GDL BTS</t>
+  </si>
+  <si>
     <t>Gilberto Perez</t>
   </si>
   <si>
@@ -303,12 +420,24 @@
     <t>MIN</t>
   </si>
   <si>
+    <t>MIN BTS</t>
+  </si>
+  <si>
     <t>Adam Hoover</t>
   </si>
   <si>
+    <t>RCH Check in lane Expansion</t>
+  </si>
+  <si>
+    <t>RIA Check in lane Expansion</t>
+  </si>
+  <si>
     <t>MIA</t>
   </si>
   <si>
+    <t>MIA Project Completion/Original Layout</t>
+  </si>
+  <si>
     <t>Concrete Repair</t>
   </si>
   <si>
@@ -318,76 +447,229 @@
     <t>COL</t>
   </si>
   <si>
+    <t>COL Dock Retro Commissioning</t>
+  </si>
+  <si>
     <t>Dock retro Fit</t>
   </si>
   <si>
+    <t>KC2 Additional Mass Handoff</t>
+  </si>
+  <si>
     <t>CAR</t>
   </si>
   <si>
+    <t>CAR Adjusting Locations For Taller Pallets</t>
+  </si>
+  <si>
     <t>PLA</t>
   </si>
   <si>
+    <t>PLA Layout Modification</t>
+  </si>
+  <si>
     <t>DA2</t>
   </si>
   <si>
+    <t>DA2 L5 CSD</t>
+  </si>
+  <si>
+    <t>GDL L2 .L3</t>
+  </si>
+  <si>
     <t>HOU</t>
   </si>
   <si>
+    <t>HOU Peason Palletizer</t>
+  </si>
+  <si>
+    <t>JAX L6 GAL with Dual Pallet Racking + L7</t>
+  </si>
+  <si>
+    <t>KC2 L2 Expansion</t>
+  </si>
+  <si>
     <t>Jacob Doerksen</t>
   </si>
   <si>
+    <t>LAN L6 (VP)</t>
+  </si>
+  <si>
+    <t>LAN L4 WIP</t>
+  </si>
+  <si>
+    <t>LAN L5</t>
+  </si>
+  <si>
+    <t>LAN L3 WIP Palletizer</t>
+  </si>
+  <si>
     <t>MES</t>
   </si>
   <si>
+    <t>MES L3</t>
+  </si>
+  <si>
+    <t>MIN L3 Precon</t>
+  </si>
+  <si>
+    <t>MXC L3</t>
+  </si>
+  <si>
+    <t>ST3 L3 GAL</t>
+  </si>
+  <si>
+    <t>ST3 Gallon Handle</t>
+  </si>
+  <si>
+    <t>TEM L4 Precon</t>
+  </si>
+  <si>
+    <t>NIA Niagara Eye</t>
+  </si>
+  <si>
     <t>Niagara Eye</t>
   </si>
   <si>
+    <t>BLM Optimization</t>
+  </si>
+  <si>
     <t>IGAL CASCOE</t>
   </si>
   <si>
     <t>NOR</t>
   </si>
   <si>
+    <t>NOR Optimization</t>
+  </si>
+  <si>
     <t>PHI</t>
   </si>
   <si>
+    <t>PHI Racking</t>
+  </si>
+  <si>
     <t>Racking Addition</t>
   </si>
   <si>
+    <t>NIA E80 Customer Service</t>
+  </si>
+  <si>
     <t>Oscar Pinto</t>
   </si>
   <si>
+    <t>RIA Pallet Inspection System</t>
+  </si>
+  <si>
     <t>BAL</t>
   </si>
   <si>
+    <t>BAL Safety V2 (Last 5)</t>
+  </si>
+  <si>
     <t>LAS</t>
   </si>
   <si>
+    <t>LAS Safety V2 (Last 5)</t>
+  </si>
+  <si>
     <t>MOR</t>
   </si>
   <si>
+    <t>MOR Safety V2 (Last 5)</t>
+  </si>
+  <si>
+    <t>NIA Safety PPDC</t>
+  </si>
+  <si>
     <t>BAK</t>
   </si>
   <si>
+    <t>BAK 18 Min Load times</t>
+  </si>
+  <si>
+    <t>BAL Rack Putaway Optimization for Pallet Height</t>
+  </si>
+  <si>
+    <t>MIN FTL/TSL WaitPreStaging Start</t>
+  </si>
+  <si>
+    <t>NIA Network Wide AutoHSK Revision</t>
+  </si>
+  <si>
+    <t>RIA Single Pallet Pick Up - FIP FIP Remote Deployment</t>
+  </si>
+  <si>
+    <t>NIA SE Project Resource Management</t>
+  </si>
+  <si>
     <t>Support</t>
   </si>
   <si>
+    <t>NIA E80 PC Priority Sheet</t>
+  </si>
+  <si>
+    <t>NIA NIA Top 10</t>
+  </si>
+  <si>
+    <t>NIA FD Matrix</t>
+  </si>
+  <si>
+    <t>HAZ Variety Pack Standarization</t>
+  </si>
+  <si>
     <t>VP Standardization</t>
   </si>
   <si>
     <t>Roger Tran</t>
   </si>
   <si>
+    <t>JAX Variety Pack Standarization</t>
+  </si>
+  <si>
+    <t>LAN Variety Pack Standarization</t>
+  </si>
+  <si>
+    <t>LOU Variety Pack Standarization</t>
+  </si>
+  <si>
+    <t>RIA Variety Pack Standarization</t>
+  </si>
+  <si>
+    <t>LAN Raw Material Segregation on Racks</t>
+  </si>
+  <si>
     <t>Weight Segregation on racks</t>
   </si>
   <si>
+    <t>DA2 L4 (GAL) + Building Expansion</t>
+  </si>
+  <si>
     <t>Building Expansion</t>
   </si>
   <si>
+    <t>MIN L3</t>
+  </si>
+  <si>
+    <t>TEM L4</t>
+  </si>
+  <si>
+    <t>HAZ Safety V1 (First 6)</t>
+  </si>
+  <si>
     <t>Complete</t>
   </si>
   <si>
     <t>Taher Poonawala</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Another</t>
   </si>
 </sst>
 </file>
@@ -478,7 +760,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -564,6 +846,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1408,8 +1693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF4A40D-63A7-47A6-905A-C1FD60372FCA}">
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="J96" sqref="J96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1466,21 +1751,20 @@
       <c r="A2" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>JAX Additional 3PL</v>
+      <c r="B2" s="31" t="s">
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="7"/>
@@ -1490,23 +1774,22 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>KC2 Dynamic Tilt Functionality Fix</v>
+        <v>39</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>40</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="7"/>
@@ -1516,23 +1799,22 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>LAN ATU Kit Addition for DA2 L5 WIP</v>
+        <v>44</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>45</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G4" s="8">
         <v>45817</v>
@@ -1550,17 +1832,16 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>OKC Shipping Gaylord with LGV</v>
+        <v>47</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>48</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1576,21 +1857,20 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>BLM Check In lane expansion</v>
+        <v>49</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>50</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="7"/>
@@ -1602,17 +1882,16 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>RCH RCH Check-In Lane: Project Planning Phase</v>
+        <v>53</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>54</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1626,23 +1905,22 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>KEN KEN -LAYOUT OPTIMIZATION</v>
+        <v>55</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>56</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="7"/>
@@ -1656,17 +1934,16 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>MIL L3 (Aluminum Line)</v>
+        <v>58</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>59</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -1678,23 +1955,22 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>HAZ Layout Opt. (Removal PBC)</v>
+        <v>61</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>62</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="7"/>
@@ -1712,19 +1988,18 @@
       <c r="A11" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>JAX Layout Opt. (Removal PBC)</v>
+      <c r="B11" s="31" t="s">
+        <v>65</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="7"/>
@@ -1736,23 +2011,22 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>RIA Layout Optimization</v>
+        <v>66</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>67</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="8">
@@ -1766,17 +2040,16 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>HAZ Implementation of Embedded</v>
+        <v>61</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>69</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -1790,17 +2063,16 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>TEM E80 Reach Optimization (Multiple sites but starting in TEM)</v>
+        <v>71</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>72</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1814,17 +2086,16 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>NIA weight Segregation roll out</v>
+        <v>73</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>74</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -1840,23 +2111,22 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>CIN S.M.I.L.E E80</v>
+        <v>75</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>76</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="G16" s="8">
         <v>45757</v>
@@ -1874,21 +2144,20 @@
       <c r="A17" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>JAX Ambient Room Automation</v>
+      <c r="B17" s="31" t="s">
+        <v>80</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="7"/>
@@ -1898,17 +2167,16 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>NIA MA Cloud Development</v>
+        <v>73</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>82</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -1924,21 +2192,20 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>ST4 Triple Stack</v>
+        <v>83</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>84</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="9"/>
@@ -1956,21 +2223,20 @@
       <c r="A20" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>JAX Dual Pallet Drive- In Racking</v>
+      <c r="B20" s="31" t="s">
+        <v>86</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G20" s="9"/>
       <c r="H20" s="7"/>
@@ -1984,17 +2250,16 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="B21" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>LOU Layout Optimization</v>
+        <v>88</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>89</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -2010,23 +2275,22 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>NIA LGV Sensor Obsolescence</v>
+        <v>73</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>90</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G22" s="9"/>
       <c r="H22" s="7"/>
@@ -2040,23 +2304,22 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>NIA LGV Sensor Obsolescence</v>
+        <v>73</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>90</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G23" s="9"/>
       <c r="H23" s="7"/>
@@ -2070,23 +2333,22 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B24" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>NIA LGV Safety Campaign</v>
+        <v>73</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>92</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G24" s="9"/>
       <c r="H24" s="7"/>
@@ -2100,17 +2362,16 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>ST4 Dual pallet Drive- in Racking</v>
+        <v>83</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>94</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -2126,23 +2387,22 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B26" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>NIA R&amp;D Sensor Retrofit Roll out - 1</v>
+        <v>73</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>95</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G26" s="9"/>
       <c r="H26" s="7"/>
@@ -2156,23 +2416,22 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>NIA R&amp;D Sensor Retrofit Roll out - 2</v>
+        <v>73</v>
+      </c>
+      <c r="B27" s="31" t="s">
+        <v>97</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G27" s="9"/>
       <c r="H27" s="7"/>
@@ -2186,24 +2445,23 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="B28" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>DAL LGV Conversion</v>
+        <v>98</v>
+      </c>
+      <c r="B28" s="31" t="s">
+        <v>99</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="9"/>
       <c r="H28" s="7"/>
       <c r="I28" s="2" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="J28" s="8">
         <v>46444</v>
@@ -2212,17 +2470,16 @@
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>NIA VP Line Optimization Roll Out</v>
+        <v>73</v>
+      </c>
+      <c r="B29" s="31" t="s">
+        <v>101</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -2238,17 +2495,16 @@
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="2" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>NIA VP Line Additiona (Line in a box)</v>
+        <v>73</v>
+      </c>
+      <c r="B30" s="31" t="s">
+        <v>102</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -2264,26 +2520,25 @@
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="B31" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>ST3 1PL</v>
+        <v>103</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>104</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="H31" s="10">
         <v>45292</v>
@@ -2300,23 +2555,22 @@
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="B32" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>BAY 3HX Exit (2 LGVs/ 3 ATU kits)</v>
+        <v>107</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E32" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="G32" s="12">
         <v>45796</v>
@@ -2332,23 +2586,22 @@
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>KC2 KC2 Injection Tote Automation</v>
+        <v>39</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G33" s="19"/>
       <c r="H33" s="11"/>
@@ -2362,26 +2615,25 @@
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>LAN Layout Opt. (PBC Removal)</v>
+        <v>44</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G34" s="16" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="H34" s="10">
         <v>45779</v>
@@ -2396,26 +2648,25 @@
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="B35" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>MXC Shipping Optimization</v>
+        <v>113</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G35" s="16" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="H35" s="11"/>
       <c r="I35" s="10">
@@ -2426,23 +2677,22 @@
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>NIA CGR03544 NIA - WIP Pallets Modification</v>
+        <v>73</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="G36" s="12">
         <v>45894</v>
@@ -2460,26 +2710,25 @@
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B37" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>NIA Monthly SE KPI</v>
+        <v>73</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="H37" s="10">
         <v>45658</v>
@@ -2494,23 +2743,22 @@
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B38" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>NIA 0 LGV Alarms</v>
+        <v>73</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G38" s="12">
         <v>45775</v>
@@ -2528,23 +2776,22 @@
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B39" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>NIA Master NIA OIL List</v>
+        <v>73</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="G39" s="19"/>
       <c r="H39" s="11"/>
@@ -2558,23 +2805,22 @@
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="B40" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>CIN BTS L1 - L3</v>
+        <v>75</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G40" s="12">
         <v>46073</v>
@@ -2592,23 +2838,22 @@
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="B41" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>GDL BTS</v>
+        <v>122</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="G41" s="12">
         <v>45769</v>
@@ -2628,23 +2873,22 @@
     </row>
     <row r="42" spans="1:11">
       <c r="A42" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="B42" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>MIN BTS</v>
+        <v>126</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>88</v>
+        <v>128</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G42" s="12">
         <v>45744</v>
@@ -2664,23 +2908,22 @@
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>RCH Check in lane Expansion</v>
+        <v>53</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G43" s="12">
         <v>45611</v>
@@ -2700,23 +2943,22 @@
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="B44" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>RIA Check in lane Expansion</v>
+        <v>66</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="G44" s="11"/>
       <c r="H44" s="10">
@@ -2734,23 +2976,22 @@
     </row>
     <row r="45" spans="1:11">
       <c r="A45" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="B45" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>MIA Project Completion/Original Layout</v>
+        <v>131</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>90</v>
+        <v>133</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G45" s="19"/>
       <c r="H45" s="11"/>
@@ -2761,28 +3002,27 @@
         <v>45688</v>
       </c>
       <c r="K45" s="18" t="s">
-        <v>91</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46" spans="1:11">
       <c r="A46" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="B46" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>COL Dock Retro Commissioning</v>
+        <v>135</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>93</v>
+        <v>137</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G46" s="12">
         <v>45798</v>
@@ -2800,23 +3040,22 @@
     </row>
     <row r="47" spans="1:11">
       <c r="A47" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B47" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>KC2 Additional Mass Handoff</v>
+        <v>39</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G47" s="19"/>
       <c r="H47" s="10">
@@ -2828,26 +3067,25 @@
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="B48" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>CAR Adjusting Locations For Taller Pallets</v>
+        <v>139</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>140</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G48" s="16" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="H48" s="10">
         <v>45775</v>
@@ -2860,23 +3098,22 @@
     </row>
     <row r="49" spans="1:11">
       <c r="A49" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="B49" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>PLA Layout Modification</v>
+        <v>141</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G49" s="10">
         <v>45775</v>
@@ -2894,23 +3131,22 @@
     </row>
     <row r="50" spans="1:11">
       <c r="A50" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="B50" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>DA2 L5 CSD</v>
+        <v>143</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E50" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F50" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="G50" s="12">
         <v>46113</v>
@@ -2926,23 +3162,22 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="B51" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>GDL L2 .L3</v>
+        <v>122</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="G51" s="12">
         <v>45982</v>
@@ -2956,26 +3191,25 @@
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="B52" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>HOU Peason Palletizer</v>
+        <v>146</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>147</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E52" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F52" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F52" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="G52" s="16" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="H52" s="10">
         <v>45579</v>
@@ -2992,21 +3226,20 @@
       <c r="A53" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B53" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>JAX L6 GAL with Dual Pallet Racking + L7</v>
+      <c r="B53" s="3" t="s">
+        <v>148</v>
       </c>
       <c r="C53" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F53" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="G53" s="12">
         <v>45734</v>
@@ -3026,23 +3259,22 @@
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B54" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>KC2 L2 Expansion</v>
+        <v>39</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>149</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>98</v>
+        <v>150</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="G54" s="10">
         <v>45845</v>
@@ -3060,23 +3292,22 @@
     </row>
     <row r="55" spans="1:11">
       <c r="A55" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B55" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>LAN L6 (VP)</v>
+        <v>44</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G55" s="12">
         <v>45517</v>
@@ -3096,23 +3327,22 @@
     </row>
     <row r="56" spans="1:11">
       <c r="A56" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B56" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>LAN L4 WIP</v>
+        <v>44</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G56" s="12">
         <v>45789</v>
@@ -3130,23 +3360,22 @@
     </row>
     <row r="57" spans="1:11">
       <c r="A57" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B57" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>LAN L5</v>
+        <v>44</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G57" s="12">
         <v>45811</v>
@@ -3164,23 +3393,22 @@
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B58" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>LAN L3 WIP Palletizer</v>
+        <v>44</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>154</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G58" s="12">
         <v>45930</v>
@@ -3198,23 +3426,22 @@
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B59" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>MES L3</v>
+        <v>155</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>156</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="G59" s="12">
         <v>45772</v>
@@ -3234,23 +3461,22 @@
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="B60" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>MIN L3 Precon</v>
+        <v>126</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="C60" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F60" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="G60" s="10">
         <v>46003</v>
@@ -3268,23 +3494,22 @@
     </row>
     <row r="61" spans="1:11">
       <c r="A61" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="B61" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>MXC L3</v>
+        <v>113</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="G61" s="12">
         <v>45755</v>
@@ -3304,23 +3529,22 @@
     </row>
     <row r="62" spans="1:11">
       <c r="A62" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="B62" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>ST3 L3 GAL</v>
+        <v>103</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>98</v>
+        <v>150</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="G62" s="12">
         <v>45703</v>
@@ -3340,23 +3564,22 @@
     </row>
     <row r="63" spans="1:11">
       <c r="A63" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="B63" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>ST3 Gallon Handle</v>
+        <v>103</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>98</v>
+        <v>150</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="G63" s="10">
         <v>45887</v>
@@ -3374,23 +3597,22 @@
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B64" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>TEM L4 Precon</v>
+        <v>71</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E64" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F64" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="G64" s="12">
         <v>45905</v>
@@ -3410,26 +3632,25 @@
     </row>
     <row r="65" spans="1:11">
       <c r="A65" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B65" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>NIA Niagara Eye</v>
+        <v>73</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>162</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>100</v>
+        <v>163</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>98</v>
+        <v>150</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="G65" s="16" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="H65" s="10">
         <v>45524</v>
@@ -3444,23 +3665,22 @@
     </row>
     <row r="66" spans="1:11">
       <c r="A66" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B66" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>BLM Optimization</v>
+        <v>49</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>164</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>101</v>
+        <v>165</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G66" s="12">
         <v>45762</v>
@@ -3478,23 +3698,22 @@
     </row>
     <row r="67" spans="1:11">
       <c r="A67" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="B67" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>NOR Optimization</v>
+        <v>166</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>101</v>
+        <v>165</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G67" s="10">
         <v>45768</v>
@@ -3512,26 +3731,25 @@
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="B68" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>PHI Racking</v>
+        <v>168</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>169</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>104</v>
+        <v>170</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="G68" s="16" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="H68" s="10">
         <v>45565</v>
@@ -3548,26 +3766,25 @@
     </row>
     <row r="69" spans="1:11">
       <c r="A69" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B69" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>NIA E80 Customer Service</v>
+        <v>73</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>171</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>105</v>
+        <v>172</v>
       </c>
       <c r="G69" s="16" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="H69" s="10">
         <v>45658</v>
@@ -3582,23 +3799,22 @@
     </row>
     <row r="70" spans="1:11">
       <c r="A70" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="B70" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>RIA Pallet Inspection System</v>
+        <v>66</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>173</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G70" s="12">
         <v>45951</v>
@@ -3616,23 +3832,22 @@
     </row>
     <row r="71" spans="1:11">
       <c r="A71" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="B71" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>BAL Safety V2 (Last 5)</v>
+        <v>174</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G71" s="10">
         <v>45817</v>
@@ -3650,23 +3865,22 @@
     </row>
     <row r="72" spans="1:11">
       <c r="A72" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="B72" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>LAS Safety V2 (Last 5)</v>
+        <v>176</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>177</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G72" s="10">
         <v>45810</v>
@@ -3684,23 +3898,22 @@
     </row>
     <row r="73" spans="1:11">
       <c r="A73" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="B73" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>MOR Safety V2 (Last 5)</v>
+        <v>178</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>179</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G73" s="10">
         <v>45810</v>
@@ -3718,23 +3931,22 @@
     </row>
     <row r="74" spans="1:11">
       <c r="A74" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B74" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>NIA Safety PPDC</v>
+        <v>73</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G74" s="19"/>
       <c r="H74" s="10">
@@ -3746,23 +3958,22 @@
     </row>
     <row r="75" spans="1:11">
       <c r="A75" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="B75" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>BAK 18 Min Load times</v>
+        <v>181</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>182</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G75" s="12">
         <v>45845</v>
@@ -3780,26 +3991,25 @@
     </row>
     <row r="76" spans="1:11">
       <c r="A76" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="B76" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>BAL Rack Putaway Optimization for Pallet Height</v>
+        <v>174</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G76" s="16" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="H76" s="10">
         <v>45743</v>
@@ -3810,23 +4020,22 @@
     </row>
     <row r="77" spans="1:11">
       <c r="A77" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="B77" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>MIN FTL/TSL WaitPreStaging Start</v>
+        <v>126</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>184</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>88</v>
+        <v>128</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G77" s="11"/>
       <c r="H77" s="11"/>
@@ -3836,23 +4045,22 @@
     </row>
     <row r="78" spans="1:11">
       <c r="A78" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B78" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>NIA Network Wide AutoHSK Revision</v>
+        <v>73</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>185</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G78" s="11"/>
       <c r="H78" s="11"/>
@@ -3862,23 +4070,22 @@
     </row>
     <row r="79" spans="1:11">
       <c r="A79" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="B79" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>RIA Single Pallet Pick Up - FIP FIP Remote Deployment</v>
+        <v>66</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>186</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G79" s="12">
         <v>45860</v>
@@ -3896,26 +4103,25 @@
     </row>
     <row r="80" spans="1:11">
       <c r="A80" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B80" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>NIA SE Project Resource Management</v>
+        <v>73</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>187</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>110</v>
+        <v>188</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>105</v>
+        <v>172</v>
       </c>
       <c r="G80" s="16" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="H80" s="10">
         <v>45658</v>
@@ -3930,26 +4136,25 @@
     </row>
     <row r="81" spans="1:11">
       <c r="A81" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B81" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>NIA E80 PC Priority Sheet</v>
+        <v>73</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>189</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>110</v>
+        <v>188</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>105</v>
+        <v>172</v>
       </c>
       <c r="G81" s="16" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="H81" s="10">
         <v>45658</v>
@@ -3964,26 +4169,25 @@
     </row>
     <row r="82" spans="1:11">
       <c r="A82" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B82" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>NIA NIA Top 10</v>
+        <v>73</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>190</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>110</v>
+        <v>188</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>105</v>
+        <v>172</v>
       </c>
       <c r="G82" s="16" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="H82" s="10">
         <v>45658</v>
@@ -3998,26 +4202,25 @@
     </row>
     <row r="83" spans="1:11">
       <c r="A83" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B83" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>NIA FD Matrix</v>
+        <v>73</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>191</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>110</v>
+        <v>188</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>105</v>
+        <v>172</v>
       </c>
       <c r="G83" s="16" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="H83" s="10">
         <v>45658</v>
@@ -4032,23 +4235,22 @@
     </row>
     <row r="84" spans="1:11">
       <c r="A84" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="B84" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>HAZ Variety Pack Standarization</v>
+        <v>61</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>111</v>
+        <v>193</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G84" s="12">
         <v>45852</v>
@@ -4068,21 +4270,20 @@
       <c r="A85" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B85" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>JAX Variety Pack Standarization</v>
+      <c r="B85" s="3" t="s">
+        <v>195</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>111</v>
+        <v>193</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G85" s="12">
         <v>45880</v>
@@ -4100,23 +4301,22 @@
     </row>
     <row r="86" spans="1:11">
       <c r="A86" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B86" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>LAN Variety Pack Standarization</v>
+        <v>44</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>196</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>111</v>
+        <v>193</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G86" s="12">
         <v>45915</v>
@@ -4134,23 +4334,22 @@
     </row>
     <row r="87" spans="1:11">
       <c r="A87" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="B87" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>LOU Variety Pack Standarization</v>
+        <v>88</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>197</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>111</v>
+        <v>193</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G87" s="12">
         <v>45943</v>
@@ -4168,23 +4367,22 @@
     </row>
     <row r="88" spans="1:11">
       <c r="A88" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="B88" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>RIA Variety Pack Standarization</v>
+        <v>66</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>198</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>111</v>
+        <v>193</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G88" s="12">
         <v>45817</v>
@@ -4202,23 +4400,22 @@
     </row>
     <row r="89" spans="1:11">
       <c r="A89" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B89" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>LAN Raw Material Segregation on Racks</v>
+        <v>44</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>199</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>113</v>
+        <v>200</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G89" s="10">
         <v>45616</v>
@@ -4236,23 +4433,22 @@
     </row>
     <row r="90" spans="1:11">
       <c r="A90" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="B90" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>DA2 L4 (GAL) + Building Expansion</v>
+        <v>143</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>201</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>114</v>
+        <v>202</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G90" s="12">
         <v>45757</v>
@@ -4272,23 +4468,22 @@
     </row>
     <row r="91" spans="1:11">
       <c r="A91" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="B91" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>MIN L3</v>
+        <v>126</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>203</v>
       </c>
       <c r="C91" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F91" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E91" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="G91" s="10">
         <v>46003</v>
@@ -4304,23 +4499,22 @@
     </row>
     <row r="92" spans="1:11">
       <c r="A92" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B92" s="3" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>TEM L4</v>
+        <v>71</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>204</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="E92" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F92" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="F92" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="G92" s="12">
         <v>45905</v>
@@ -4336,23 +4530,22 @@
     </row>
     <row r="93" spans="1:11">
       <c r="A93" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="B93" s="4" t="str">
-        <f ca="1">CONCATENATE(Table3[[#This Row],[Plant]]," ", Table3[[#This Row],[Project Name]])</f>
-        <v>HAZ Safety V1 (First 6)</v>
+        <v>61</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>205</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>115</v>
+        <v>206</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>116</v>
+        <v>207</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="G93" s="21">
         <v>45481</v>
@@ -4367,28 +4560,60 @@
       <c r="K93" s="22"/>
     </row>
     <row r="94" spans="1:11">
-      <c r="A94" s="26"/>
-      <c r="B94" s="27"/>
-      <c r="C94" s="28"/>
-      <c r="D94" s="28"/>
-      <c r="E94" s="5"/>
-      <c r="F94" s="28"/>
+      <c r="A94" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="B94" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="C94" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="D94" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F94" s="28" t="s">
+        <v>79</v>
+      </c>
       <c r="G94" s="30"/>
       <c r="H94" s="29"/>
-      <c r="I94" s="29"/>
-      <c r="J94" s="17"/>
+      <c r="I94" s="29">
+        <v>45662</v>
+      </c>
+      <c r="J94" s="17">
+        <v>45667</v>
+      </c>
       <c r="K94" s="18"/>
     </row>
     <row r="95" spans="1:11">
-      <c r="A95" s="26"/>
-      <c r="B95" s="27"/>
-      <c r="C95" s="28"/>
-      <c r="D95" s="28"/>
-      <c r="E95" s="5"/>
-      <c r="F95" s="28"/>
+      <c r="A95" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="B95" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="C95" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="D95" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F95" s="28" t="s">
+        <v>79</v>
+      </c>
       <c r="H95" s="29"/>
-      <c r="I95" s="29"/>
-      <c r="J95" s="17"/>
+      <c r="I95" s="29">
+        <v>45693</v>
+      </c>
+      <c r="J95" s="17">
+        <v>45726</v>
+      </c>
       <c r="K95" s="18"/>
     </row>
     <row r="96" spans="1:11">

</xml_diff>